<commit_message>
[Fixed] toLowerCase materia prima productos name
</commit_message>
<xml_diff>
--- a/formatos/formato-distribucion-directa.xlsx
+++ b/formatos/formato-distribucion-directa.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF06BC61-9497-4100-9934-EBD85A97DC94}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B5C0631-B109-4192-9186-BEDE237B0B58}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Gastos Generales" sheetId="1" r:id="rId1"/>
+    <sheet name="Distribucion" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -386,7 +386,7 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>